<commit_message>
Import events form (#6)
* event imports

WIP

get parsing working

import table

finish event import table etc

fix weird select behavior

add event import endpoint

refactor events API

update ToggleInput

fix label

required fields and styling fixes

remove outdated slate package

* regenerate package.lock after crazy rebase

* descriptions

* X button to remove select choice

* cleanup
</commit_message>
<xml_diff>
--- a/data/people-100.xlsx
+++ b/data/people-100.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lorinjameson/Work/AVAnnotate/admin-client/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/camden/Documents/code/admin-client/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{54E92D5A-E858-3C44-900A-146D5AD61B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B6634E-0624-BD41-854F-EE56B7B1C67F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4480" yWindow="2700" windowWidth="27640" windowHeight="16940" xr2:uid="{02DC3CC2-EAD9-E54D-BBBD-C6B109FB7C40}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="581">
   <si>
     <t>Index</t>
   </si>
@@ -1770,13 +1770,19 @@
   </si>
   <si>
     <t>IT sales professional</t>
+  </si>
+  <si>
+    <t>Item Type</t>
+  </si>
+  <si>
+    <t>Audio</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2631,13 +2637,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E77444A-3643-934B-ABEA-3C64B1B39F0B}">
-  <dimension ref="A1:I101"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L94" sqref="L94"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="9" max="9" width="20.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2665,8 +2676,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2694,8 +2708,11 @@
       <c r="I2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2723,8 +2740,11 @@
       <c r="I3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2752,8 +2772,11 @@
       <c r="I4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2781,8 +2804,11 @@
       <c r="I5" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2810,8 +2836,11 @@
       <c r="I6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2839,8 +2868,11 @@
       <c r="I7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2868,8 +2900,11 @@
       <c r="I8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2897,8 +2932,11 @@
       <c r="I9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2926,8 +2964,11 @@
       <c r="I10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2955,8 +2996,11 @@
       <c r="I11" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2984,8 +3028,11 @@
       <c r="I12" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3013,8 +3060,11 @@
       <c r="I13" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3042,8 +3092,11 @@
       <c r="I14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3071,8 +3124,11 @@
       <c r="I15" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3101,8 +3157,11 @@
       <c r="I16" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3131,8 +3190,11 @@
       <c r="I17" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>17</v>
       </c>
@@ -3160,8 +3222,11 @@
       <c r="I18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>18</v>
       </c>
@@ -3189,8 +3254,11 @@
       <c r="I19" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3218,8 +3286,11 @@
       <c r="I20" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3248,8 +3319,11 @@
       <c r="I21" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3277,8 +3351,11 @@
       <c r="I22" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3306,8 +3383,11 @@
       <c r="I23" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3335,8 +3415,11 @@
       <c r="I24" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3364,8 +3447,11 @@
       <c r="I25" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3393,8 +3479,11 @@
       <c r="I26" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3422,8 +3511,11 @@
       <c r="I27" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3451,8 +3543,11 @@
       <c r="I28" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3480,8 +3575,11 @@
       <c r="I29" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3509,8 +3607,11 @@
       <c r="I30" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3538,8 +3639,11 @@
       <c r="I31" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3567,8 +3671,11 @@
       <c r="I32" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3596,8 +3703,11 @@
       <c r="I33" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3625,8 +3735,11 @@
       <c r="I34" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3654,8 +3767,11 @@
       <c r="I35" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3683,8 +3799,11 @@
       <c r="I36" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3712,8 +3831,11 @@
       <c r="I37" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3741,8 +3863,11 @@
       <c r="I38" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3770,8 +3895,11 @@
       <c r="I39" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>39</v>
       </c>
@@ -3799,8 +3927,11 @@
       <c r="I40" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>40</v>
       </c>
@@ -3828,8 +3959,11 @@
       <c r="I41" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3857,8 +3991,11 @@
       <c r="I42" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3886,8 +4023,11 @@
       <c r="I43" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3915,8 +4055,11 @@
       <c r="I44" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3944,8 +4087,11 @@
       <c r="I45" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3973,8 +4119,11 @@
       <c r="I46" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4002,8 +4151,11 @@
       <c r="I47" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4031,8 +4183,11 @@
       <c r="I48" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4060,8 +4215,11 @@
       <c r="I49" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4089,8 +4247,11 @@
       <c r="I50" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4118,8 +4279,11 @@
       <c r="I51" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
       <c r="A52">
         <v>51</v>
       </c>
@@ -4147,8 +4311,11 @@
       <c r="I52" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
       <c r="A53">
         <v>52</v>
       </c>
@@ -4176,8 +4343,11 @@
       <c r="I53" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
       <c r="A54">
         <v>53</v>
       </c>
@@ -4205,8 +4375,11 @@
       <c r="I54" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
       <c r="A55">
         <v>54</v>
       </c>
@@ -4234,8 +4407,11 @@
       <c r="I55" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
       <c r="A56">
         <v>55</v>
       </c>
@@ -4263,8 +4439,11 @@
       <c r="I56" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
       <c r="A57">
         <v>56</v>
       </c>
@@ -4292,8 +4471,11 @@
       <c r="I57" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
       <c r="A58">
         <v>57</v>
       </c>
@@ -4321,8 +4503,11 @@
       <c r="I58" t="s">
         <v>337</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
       <c r="A59">
         <v>58</v>
       </c>
@@ -4350,8 +4535,11 @@
       <c r="I59" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4379,8 +4567,11 @@
       <c r="I60" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4408,8 +4599,11 @@
       <c r="I61" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J61" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4437,8 +4631,11 @@
       <c r="I62" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J62" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4466,8 +4663,11 @@
       <c r="I63" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J63" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4495,8 +4695,11 @@
       <c r="I64" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J64" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4524,8 +4727,11 @@
       <c r="I65" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J65" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>65</v>
       </c>
@@ -4554,8 +4760,11 @@
       <c r="I66" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J66" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>66</v>
       </c>
@@ -4583,8 +4792,11 @@
       <c r="I67" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J67" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>67</v>
       </c>
@@ -4612,8 +4824,11 @@
       <c r="I68" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J68" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>68</v>
       </c>
@@ -4641,8 +4856,11 @@
       <c r="I69" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>69</v>
       </c>
@@ -4670,8 +4888,11 @@
       <c r="I70" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>70</v>
       </c>
@@ -4699,8 +4920,11 @@
       <c r="I71" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>71</v>
       </c>
@@ -4728,8 +4952,11 @@
       <c r="I72" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J72" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>72</v>
       </c>
@@ -4757,8 +4984,11 @@
       <c r="I73" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J73" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>73</v>
       </c>
@@ -4786,8 +5016,11 @@
       <c r="I74" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J74" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>74</v>
       </c>
@@ -4815,8 +5048,11 @@
       <c r="I75" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J75" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
       <c r="A76">
         <v>75</v>
       </c>
@@ -4844,8 +5080,11 @@
       <c r="I76" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J76" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
       <c r="A77">
         <v>76</v>
       </c>
@@ -4873,8 +5112,11 @@
       <c r="I77" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J77" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
       <c r="A78">
         <v>77</v>
       </c>
@@ -4902,8 +5144,11 @@
       <c r="I78" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J78" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
       <c r="A79">
         <v>78</v>
       </c>
@@ -4931,8 +5176,11 @@
       <c r="I79" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J79" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
       <c r="A80">
         <v>79</v>
       </c>
@@ -4960,8 +5208,11 @@
       <c r="I80" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
       <c r="A81">
         <v>80</v>
       </c>
@@ -4989,8 +5240,11 @@
       <c r="I81" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
       <c r="A82">
         <v>81</v>
       </c>
@@ -5018,8 +5272,11 @@
       <c r="I82" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
       <c r="A83">
         <v>82</v>
       </c>
@@ -5047,8 +5304,11 @@
       <c r="I83" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
       <c r="A84">
         <v>83</v>
       </c>
@@ -5076,8 +5336,11 @@
       <c r="I84" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
       <c r="A85">
         <v>84</v>
       </c>
@@ -5105,8 +5368,11 @@
       <c r="I85" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10">
       <c r="A86">
         <v>85</v>
       </c>
@@ -5134,8 +5400,11 @@
       <c r="I86" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10">
       <c r="A87">
         <v>86</v>
       </c>
@@ -5163,8 +5432,11 @@
       <c r="I87" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10">
       <c r="A88">
         <v>87</v>
       </c>
@@ -5192,8 +5464,11 @@
       <c r="I88" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J88" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10">
       <c r="A89">
         <v>88</v>
       </c>
@@ -5221,8 +5496,11 @@
       <c r="I89" t="s">
         <v>512</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J89" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10">
       <c r="A90">
         <v>89</v>
       </c>
@@ -5251,8 +5529,11 @@
       <c r="I90" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J90" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10">
       <c r="A91">
         <v>90</v>
       </c>
@@ -5280,8 +5561,11 @@
       <c r="I91" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10">
       <c r="A92">
         <v>91</v>
       </c>
@@ -5309,8 +5593,11 @@
       <c r="I92" t="s">
         <v>528</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J92" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10">
       <c r="A93">
         <v>92</v>
       </c>
@@ -5338,8 +5625,11 @@
       <c r="I93" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10">
       <c r="A94">
         <v>93</v>
       </c>
@@ -5367,8 +5657,11 @@
       <c r="I94" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J94" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10">
       <c r="A95">
         <v>94</v>
       </c>
@@ -5396,8 +5689,11 @@
       <c r="I95" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10">
       <c r="A96">
         <v>95</v>
       </c>
@@ -5425,8 +5721,11 @@
       <c r="I96" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10">
       <c r="A97">
         <v>96</v>
       </c>
@@ -5454,8 +5753,11 @@
       <c r="I97" t="s">
         <v>555</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J97" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10">
       <c r="A98">
         <v>97</v>
       </c>
@@ -5483,8 +5785,11 @@
       <c r="I98" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10">
       <c r="A99">
         <v>98</v>
       </c>
@@ -5512,8 +5817,11 @@
       <c r="I99" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10">
       <c r="A100">
         <v>99</v>
       </c>
@@ -5541,8 +5849,11 @@
       <c r="I100" t="s">
         <v>572</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J100" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10">
       <c r="A101">
         <v>100</v>
       </c>
@@ -5569,6 +5880,9 @@
       </c>
       <c r="I101" t="s">
         <v>578</v>
+      </c>
+      <c r="J101" t="s">
+        <v>580</v>
       </c>
     </row>
   </sheetData>

</xml_diff>